<commit_message>
post and delete files added with runner and allure reports
</commit_message>
<xml_diff>
--- a/7CRUDCarriers_LMS_API/src/test/resources/excelData/program_testdata.xlsx
+++ b/7CRUDCarriers_LMS_API/src/test/resources/excelData/program_testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavit\eclipse-workspace\7CRUDCarriers_LMS_API\src\test\resources\excelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavit\git\7CRUDCarriers_LMS_API\7CRUDCarriers_LMS_API\src\test\resources\excelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1636F33D-A8D1-402D-B0FF-DFB0F30BF1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22436E90-8B4F-46FC-8C3B-C82920B7C3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="get" sheetId="4" r:id="rId1"/>
@@ -23,14 +23,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="83">
   <si>
     <t>Test case Name</t>
   </si>
   <si>
-    <t>Check if user is able to create new User Record</t>
-  </si>
-  <si>
     <t>To create record with invalid linkedin url</t>
   </si>
   <si>
@@ -100,21 +97,6 @@
     <t>To update visa status with invalid input</t>
   </si>
   <si>
-    <t>To delete the user id with existing user id</t>
-  </si>
-  <si>
-    <t>404</t>
-  </si>
-  <si>
-    <t>Not Found</t>
-  </si>
-  <si>
-    <t>To delete the user with invalid user id</t>
-  </si>
-  <si>
-    <t>U72</t>
-  </si>
-  <si>
     <t>1.23</t>
   </si>
   <si>
@@ -122,9 +104,6 @@
   </si>
   <si>
     <t>User successfully Created!</t>
-  </si>
-  <si>
-    <t>To create user record with visa status and location blank</t>
   </si>
   <si>
     <t>{
@@ -164,26 +143,6 @@
     <t>User Successfully Updated</t>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>To delete the user id with non-existing user id</t>
-  </si>
-  <si>
-    <t>Deleted</t>
-  </si>
-  <si>
-    <t>{
-"name": "Shilpa,Patel",
-"phone_number": 9120006788,
-"time_zone": "EST",
-"linkedin_url": "https://www.linkedin.com/in/Patel/",
-"education_ug": "Electronic Engineering",
-"education_pg": "MBA",
-"comments": "Hello"
-}</t>
-  </si>
-  <si>
     <t>{
 "name": ",Zinta",
 "phone_number": 1234557890,
@@ -205,19 +164,6 @@
 "linkedin_url": "https://www.linkedin.com/in/Siara/",
 "education_ug": "Computer Science Engineering",
 "education_pg": "MBA",
-"visa_status": "Not-Specified",
-"comments": "Hello"
-}</t>
-  </si>
-  <si>
-    <t>{
-"name": "Ruchi,Dcruz",
-"phone_number": 4298490488,
-"location": "seattle",
-"time_zone": "EST",
-"linkedin_url": "https://www.linkedin.com/in/Ruchi Dcruz/",
-"education_ug": "Computer Science Engineering",
-"education_pg": " MBA",
 "visa_status": "Not-Specified",
 "comments": "Hello"
 }</t>
@@ -301,9 +247,6 @@
 }  </t>
   </si>
   <si>
-    <t>To create User with duplicate record</t>
-  </si>
-  <si>
     <t>To create User record with blank linkedin_url, education_pg, comments</t>
   </si>
   <si>
@@ -422,9 +365,6 @@
 }</t>
   </si>
   <si>
-    <t>U156</t>
-  </si>
-  <si>
     <t>ProgramId</t>
   </si>
   <si>
@@ -453,13 +393,86 @@
   </si>
   <si>
     <t>Null</t>
+  </si>
+  <si>
+    <t>520</t>
+  </si>
+  <si>
+    <t>Check if the user able to create new Program</t>
+  </si>
+  <si>
+    <t>{
+        "programName": "Jan23-CRUDCarriers-SDET-50",
+        "programDescription": "Update Program By Name null",
+        "programStatus": "InActive",
+        "creationTime": "2023-01-11T02:00:02.628+00:00",
+        "lastModTime": "2023-01-11T02:00:02.628+00:00"}</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>Program  successfully Created!</t>
+  </si>
+  <si>
+    <t>{
+   "programName": "",
+        "programDescription": "",
+        "programStatus": "",
+        "creationTime": "",
+        "lastModTime": ""
+}</t>
+  </si>
+  <si>
+    <t>Create new Program with duplicate record</t>
+  </si>
+  <si>
+    <t>To create user record with blank fields</t>
+  </si>
+  <si>
+    <t>To delete existing program by id</t>
+  </si>
+  <si>
+    <t>Deleted Successfully</t>
+  </si>
+  <si>
+    <t>To delete existing program by name</t>
+  </si>
+  <si>
+    <t>To delete non-existing program by id</t>
+  </si>
+  <si>
+    <t>Bad Request</t>
+  </si>
+  <si>
+    <t>To delete non-existing program by name</t>
+  </si>
+  <si>
+    <t>Java267</t>
+  </si>
+  <si>
+    <t>To delete the program without passing the program id or name</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>{
+        "programName": "Jan23-CRUDCarriers-SDET-562",
+        "programDescription": "Update Program By Name null",
+        "programStatus": "InActive",
+        "creationTime": "2023-01-11T02:00:02.628+00:00",
+        "lastModTime": "2023-01-11T02:00:02.628+00:00"}</t>
+  </si>
+  <si>
+    <t>Jan23-CRUDCarriers-SDET-562</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,6 +487,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0451A5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -490,7 +515,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -513,11 +538,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -532,9 +617,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -557,11 +639,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -856,80 +962,80 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>9</v>
+        <v>56</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="15">
-        <v>520</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>9</v>
+        <v>57</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>13</v>
+        <v>58</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>13</v>
+        <v>62</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>13</v>
+        <v>63</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>13</v>
+        <v>61</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="16">
+        <v>59</v>
+      </c>
+      <c r="C8" s="14">
         <v>404</v>
       </c>
     </row>
@@ -944,7 +1050,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,181 +1066,181 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1165,152 +1271,152 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="B3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="216" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="216" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="E3" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="216" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="B6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="B7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="216" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="B8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>18</v>
+      <c r="B9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1323,126 +1429,141 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="22">
+        <v>2548</v>
+      </c>
+      <c r="C2" s="16">
+        <v>200</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="20">
+        <v>200</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="23">
+        <v>6000</v>
+      </c>
+      <c r="C4" s="20">
+        <v>400</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="20">
+        <v>400</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="20">
+        <v>404</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>